<commit_message>
Working through knitting errors in completed R final project
</commit_message>
<xml_diff>
--- a/case_study_table.xlsx
+++ b/case_study_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashaedmondson/Desktop/Environmental_Data_Analytics_2020/FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{608DFDAC-6737-C44E-BB38-66732AC1C59E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEC80B2-83CF-714C-AC8A-105A1B01B8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="2160" windowWidth="25440" windowHeight="14320" xr2:uid="{F8822168-8648-D543-98D3-2E7B70E3E9EB}"/>
+    <workbookView xWindow="160" yWindow="580" windowWidth="25440" windowHeight="14320" xr2:uid="{F8822168-8648-D543-98D3-2E7B70E3E9EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,15 +38,6 @@
     <t>County</t>
   </si>
   <si>
-    <t>Data_samples</t>
-  </si>
-  <si>
-    <t>Highest_fecal_coliform_concentration</t>
-  </si>
-  <si>
-    <t>units_measured</t>
-  </si>
-  <si>
     <t>Greene</t>
   </si>
   <si>
@@ -65,21 +56,38 @@
     <t>Wayne</t>
   </si>
   <si>
-    <t>County_code</t>
-  </si>
-  <si>
-    <t>Monitoring_Sites</t>
-  </si>
-  <si>
     <t>cfu/100ml</t>
+  </si>
+  <si>
+    <t>County code</t>
+  </si>
+  <si>
+    <t>Monitoring Sites</t>
+  </si>
+  <si>
+    <t>Data Samples</t>
+  </si>
+  <si>
+    <t>Highest Fecal Coliform Concentration</t>
+  </si>
+  <si>
+    <t>Units Measured</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,8 +115,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,149 +441,155 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="34">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" s="3">
+        <v>79</v>
+      </c>
+      <c r="C2" s="3">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1403</v>
+      </c>
+      <c r="E2" s="3">
+        <v>140000</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3" s="3">
+        <v>147</v>
+      </c>
+      <c r="C3" s="3">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3425</v>
+      </c>
+      <c r="E3" s="3">
+        <v>190000</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B4" s="3">
+        <v>61</v>
+      </c>
+      <c r="C4" s="3">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3128</v>
+      </c>
+      <c r="E4" s="3">
+        <v>820000</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>79</v>
-      </c>
-      <c r="C2">
-        <v>16</v>
-      </c>
-      <c r="D2">
-        <v>1403</v>
-      </c>
-      <c r="E2">
-        <v>140000</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5" s="3">
+        <v>107</v>
+      </c>
+      <c r="C5" s="3">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2047</v>
+      </c>
+      <c r="E5" s="3">
+        <v>40000</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>147</v>
-      </c>
-      <c r="C3">
-        <v>56</v>
-      </c>
-      <c r="D3">
-        <v>3425</v>
-      </c>
-      <c r="E3">
-        <v>190000</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B6" s="3">
+        <v>163</v>
+      </c>
+      <c r="C6" s="3">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2836</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>61</v>
-      </c>
-      <c r="C4">
-        <v>58</v>
-      </c>
-      <c r="D4">
-        <v>3128</v>
-      </c>
-      <c r="E4">
+      <c r="B7" s="3">
+        <v>191</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2121</v>
+      </c>
+      <c r="E7" s="3">
         <v>820000</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="F7" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B5">
-        <v>107</v>
-      </c>
-      <c r="C5">
-        <v>28</v>
-      </c>
-      <c r="D5">
-        <v>2047</v>
-      </c>
-      <c r="E5">
-        <v>40000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>163</v>
-      </c>
-      <c r="C6">
-        <v>46</v>
-      </c>
-      <c r="D6">
-        <v>2836</v>
-      </c>
-      <c r="E6">
-        <v>1000000</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>191</v>
-      </c>
-      <c r="C7">
-        <v>45</v>
-      </c>
-      <c r="D7">
-        <v>2121</v>
-      </c>
-      <c r="E7">
-        <v>820000</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>